<commit_message>
Added 'Calibrate?' column to parameters sheet
</commit_message>
<xml_diff>
--- a/project/cascade-belarus.xlsx
+++ b/project/cascade-belarus.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjarvis/git/tb-ucl/project/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="984" yWindow="180" windowWidth="23256" windowHeight="13116" activeTab="3"/>
+    <workbookView xWindow="-5400" yWindow="-23220" windowWidth="35020" windowHeight="20860" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Sheet Names" sheetId="5" r:id="rId1"/>
@@ -16,6 +21,9 @@
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -82,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="577">
   <si>
     <t>Code Label</t>
   </si>
@@ -1976,6 +1984,9 @@
   </si>
   <si>
     <t>Disaggregation Ratios</t>
+  </si>
+  <si>
+    <t>Calibrate?</t>
   </si>
 </sst>
 </file>
@@ -2851,13 +2862,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>325120</xdr:colOff>
       <xdr:row>104</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>155316</xdr:colOff>
       <xdr:row>111</xdr:row>
       <xdr:rowOff>156633</xdr:rowOff>
@@ -3183,13 +3194,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>79</v>
       </c>
@@ -3197,7 +3208,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>81</v>
       </c>
@@ -3205,7 +3216,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>403</v>
       </c>
@@ -3213,7 +3224,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>82</v>
       </c>
@@ -3221,7 +3232,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>276</v>
       </c>
@@ -3229,7 +3240,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>84</v>
       </c>
@@ -3237,7 +3248,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>559</v>
       </c>
@@ -3245,7 +3256,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>539</v>
       </c>
@@ -3253,7 +3264,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>573</v>
       </c>
@@ -3261,7 +3272,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>538</v>
       </c>
@@ -3269,7 +3280,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>574</v>
       </c>
@@ -3277,7 +3288,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>556</v>
       </c>
@@ -3285,7 +3296,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>277</v>
       </c>
@@ -3293,7 +3304,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>343</v>
       </c>
@@ -3303,11 +3314,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3319,17 +3325,17 @@
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="8.77734375" style="2"/>
+    <col min="4" max="4" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3352,7 +3358,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3363,7 +3369,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3374,7 +3380,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>206</v>
       </c>
@@ -3385,7 +3391,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>207</v>
       </c>
@@ -3396,7 +3402,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>208</v>
       </c>
@@ -3407,7 +3413,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>209</v>
       </c>
@@ -3418,7 +3424,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>210</v>
       </c>
@@ -3429,7 +3435,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>211</v>
       </c>
@@ -3440,7 +3446,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>75</v>
       </c>
@@ -3451,7 +3457,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>203</v>
       </c>
@@ -3465,7 +3471,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>204</v>
       </c>
@@ -3479,7 +3485,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>127</v>
       </c>
@@ -3490,7 +3496,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -3501,7 +3507,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>129</v>
       </c>
@@ -3512,7 +3518,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>130</v>
       </c>
@@ -3523,7 +3529,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>131</v>
       </c>
@@ -3534,7 +3540,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>132</v>
       </c>
@@ -3545,7 +3551,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>133</v>
       </c>
@@ -3556,7 +3562,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>134</v>
       </c>
@@ -3567,7 +3573,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>135</v>
       </c>
@@ -3578,7 +3584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>205</v>
       </c>
@@ -3592,7 +3598,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>136</v>
       </c>
@@ -3603,7 +3609,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>137</v>
       </c>
@@ -3614,7 +3620,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>138</v>
       </c>
@@ -3625,7 +3631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>139</v>
       </c>
@@ -3636,7 +3642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>140</v>
       </c>
@@ -3647,7 +3653,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>141</v>
       </c>
@@ -3658,7 +3664,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>142</v>
       </c>
@@ -3669,7 +3675,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -3680,7 +3686,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -3691,7 +3697,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>76</v>
       </c>
@@ -3702,7 +3708,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -3716,7 +3722,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -3730,7 +3736,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>270</v>
       </c>
@@ -3746,11 +3752,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3762,44 +3763,44 @@
       <selection activeCell="AJ20" sqref="AJ20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.33203125" customWidth="1"/>
-    <col min="4" max="4" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5.33203125" customWidth="1"/>
     <col min="15" max="15" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="5.33203125" customWidth="1"/>
     <col min="25" max="25" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="7" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="4.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>270</v>
@@ -3904,7 +3905,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>270</v>
       </c>
@@ -3947,7 +3948,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -3992,7 +3993,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -4035,7 +4036,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>206</v>
       </c>
@@ -4082,7 +4083,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>207</v>
       </c>
@@ -4129,7 +4130,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>208</v>
       </c>
@@ -4174,7 +4175,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>209</v>
       </c>
@@ -4219,7 +4220,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>210</v>
       </c>
@@ -4264,7 +4265,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
         <v>211</v>
       </c>
@@ -4309,7 +4310,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>75</v>
       </c>
@@ -4352,7 +4353,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>203</v>
       </c>
@@ -4395,7 +4396,7 @@
       <c r="AH12" s="20"/>
       <c r="AI12" s="22"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>204</v>
       </c>
@@ -4440,7 +4441,7 @@
       <c r="AH13" s="10"/>
       <c r="AI13" s="11"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>127</v>
       </c>
@@ -4487,7 +4488,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>128</v>
       </c>
@@ -4534,7 +4535,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>129</v>
       </c>
@@ -4583,7 +4584,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>130</v>
       </c>
@@ -4630,7 +4631,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>131</v>
       </c>
@@ -4677,7 +4678,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>132</v>
       </c>
@@ -4726,7 +4727,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>133</v>
       </c>
@@ -4773,7 +4774,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>134</v>
       </c>
@@ -4820,7 +4821,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>135</v>
       </c>
@@ -4867,7 +4868,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>205</v>
       </c>
@@ -4912,7 +4913,7 @@
       <c r="AH23" s="7"/>
       <c r="AI23" s="8"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>136</v>
       </c>
@@ -4959,7 +4960,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>137</v>
       </c>
@@ -5006,7 +5007,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>138</v>
       </c>
@@ -5055,7 +5056,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>139</v>
       </c>
@@ -5102,7 +5103,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>140</v>
       </c>
@@ -5149,7 +5150,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>141</v>
       </c>
@@ -5198,7 +5199,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>142</v>
       </c>
@@ -5245,7 +5246,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>143</v>
       </c>
@@ -5292,7 +5293,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>144</v>
       </c>
@@ -5339,7 +5340,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>76</v>
       </c>
@@ -5382,7 +5383,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>41</v>
       </c>
@@ -5421,7 +5422,7 @@
       <c r="AH34" s="10"/>
       <c r="AI34" s="11"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>42</v>
       </c>
@@ -5464,11 +5465,6 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5477,35 +5473,35 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="56.6640625" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="16" width="8.77734375" customWidth="1"/>
+    <col min="12" max="16" width="8.83203125" customWidth="1"/>
     <col min="17" max="18" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5537,7 +5533,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -5550,6 +5546,9 @@
       <c r="D2" s="2">
         <v>-1</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>433</v>
+      </c>
       <c r="J2" t="s">
         <v>206</v>
       </c>
@@ -5569,7 +5568,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -5582,9 +5581,6 @@
       <c r="D3" s="2">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>433</v>
-      </c>
       <c r="J3" t="s">
         <v>127</v>
       </c>
@@ -5592,7 +5588,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>146</v>
       </c>
@@ -5615,7 +5611,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>147</v>
       </c>
@@ -5638,7 +5634,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -5661,7 +5657,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>175</v>
       </c>
@@ -5684,7 +5680,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>176</v>
       </c>
@@ -5707,7 +5703,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>148</v>
       </c>
@@ -5745,7 +5741,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>177</v>
       </c>
@@ -5783,7 +5779,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -5796,6 +5792,9 @@
       <c r="D11" s="2">
         <v>1</v>
       </c>
+      <c r="F11" s="2" t="s">
+        <v>433</v>
+      </c>
       <c r="J11" t="s">
         <v>203</v>
       </c>
@@ -5806,7 +5805,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -5844,7 +5843,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -5870,7 +5869,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>149</v>
       </c>
@@ -5896,7 +5895,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>150</v>
       </c>
@@ -5922,7 +5921,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>151</v>
       </c>
@@ -5948,7 +5947,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>178</v>
       </c>
@@ -5974,7 +5973,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>179</v>
       </c>
@@ -6001,7 +6000,7 @@
       </c>
       <c r="O18" s="15"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>180</v>
       </c>
@@ -6027,7 +6026,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>152</v>
       </c>
@@ -6056,7 +6055,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>181</v>
       </c>
@@ -6085,7 +6084,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -6111,7 +6110,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>327</v>
       </c>
@@ -6128,7 +6127,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>332</v>
       </c>
@@ -6151,7 +6150,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>331</v>
       </c>
@@ -6174,7 +6173,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>328</v>
       </c>
@@ -6191,7 +6190,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>330</v>
       </c>
@@ -6211,7 +6210,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>335</v>
       </c>
@@ -6237,7 +6236,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>333</v>
       </c>
@@ -6260,7 +6259,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>334</v>
       </c>
@@ -6286,7 +6285,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>365</v>
       </c>
@@ -6306,7 +6305,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>375</v>
       </c>
@@ -6332,7 +6331,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>376</v>
       </c>
@@ -6358,7 +6357,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>377</v>
       </c>
@@ -6384,7 +6383,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>372</v>
       </c>
@@ -6410,7 +6409,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>373</v>
       </c>
@@ -6436,7 +6435,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>374</v>
       </c>
@@ -6462,7 +6461,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>367</v>
       </c>
@@ -6488,7 +6487,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>366</v>
       </c>
@@ -6514,7 +6513,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>368</v>
       </c>
@@ -6540,7 +6539,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>382</v>
       </c>
@@ -6557,7 +6556,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>383</v>
       </c>
@@ -6574,7 +6573,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>384</v>
       </c>
@@ -6588,7 +6587,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>385</v>
       </c>
@@ -6609,7 +6608,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>386</v>
       </c>
@@ -6630,7 +6629,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>387</v>
       </c>
@@ -6651,7 +6650,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>388</v>
       </c>
@@ -6672,7 +6671,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>389</v>
       </c>
@@ -6693,7 +6692,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>390</v>
       </c>
@@ -6714,7 +6713,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>391</v>
       </c>
@@ -6740,7 +6739,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>392</v>
       </c>
@@ -6766,7 +6765,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>393</v>
       </c>
@@ -6791,37 +6790,33 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N107"/>
+  <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="118.109375" style="23" customWidth="1"/>
-    <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="9" width="98" customWidth="1"/>
-    <col min="14" max="14" width="75.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10" style="2" customWidth="1"/>
+    <col min="8" max="8" width="118.1640625" style="23" customWidth="1"/>
+    <col min="9" max="9" width="40" customWidth="1"/>
+    <col min="10" max="10" width="98" customWidth="1"/>
+    <col min="15" max="15" width="75.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -6841,16 +6836,19 @@
         <v>63</v>
       </c>
       <c r="G1" s="15" t="s">
+        <v>576</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -6867,11 +6865,14 @@
       <c r="F2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I2" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>316</v>
       </c>
@@ -6886,14 +6887,14 @@
       <c r="F3" s="2">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>297</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="J3" s="23" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>301</v>
       </c>
@@ -6910,14 +6911,14 @@
       <c r="F4" s="2">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>313</v>
       </c>
-      <c r="I4" s="50" t="s">
+      <c r="J4" s="50" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>317</v>
       </c>
@@ -6934,14 +6935,14 @@
       <c r="F5" s="2">
         <v>4</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>299</v>
       </c>
-      <c r="I5" s="50" t="s">
+      <c r="J5" s="50" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>318</v>
       </c>
@@ -6958,14 +6959,14 @@
       <c r="F6" s="2">
         <v>5</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>300</v>
       </c>
-      <c r="I6" s="50" t="s">
+      <c r="J6" s="50" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>222</v>
       </c>
@@ -6978,12 +6979,15 @@
       <c r="F7" s="2">
         <v>-1</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H7" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>232</v>
       </c>
@@ -6996,11 +7000,14 @@
       <c r="F8" s="2">
         <v>-1</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H8" s="23" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>233</v>
       </c>
@@ -7013,11 +7020,14 @@
       <c r="F9" s="2">
         <v>-1</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H9" s="23" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>234</v>
       </c>
@@ -7030,11 +7040,14 @@
       <c r="F10" s="2">
         <v>-1</v>
       </c>
-      <c r="G10" s="23" t="s">
+      <c r="G10" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H10" s="23" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>225</v>
       </c>
@@ -7047,11 +7060,14 @@
       <c r="F11" s="2">
         <v>-1</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H11" s="23" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>235</v>
       </c>
@@ -7064,11 +7080,14 @@
       <c r="F12" s="2">
         <v>-1</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H12" s="23" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>236</v>
       </c>
@@ -7081,11 +7100,14 @@
       <c r="F13" s="2">
         <v>-1</v>
       </c>
-      <c r="G13" s="23" t="s">
+      <c r="G13" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H13" s="23" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>237</v>
       </c>
@@ -7098,16 +7120,19 @@
       <c r="F14" s="2">
         <v>-1</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H14" s="23" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="D15"/>
-      <c r="I15" s="50"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="50"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>312</v>
       </c>
@@ -7121,14 +7146,14 @@
       <c r="E16" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>314</v>
       </c>
-      <c r="I16" s="49" t="s">
+      <c r="J16" s="49" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>292</v>
       </c>
@@ -7142,14 +7167,14 @@
       <c r="E17" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>315</v>
       </c>
-      <c r="I17" s="52" t="s">
+      <c r="J17" s="52" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>295</v>
       </c>
@@ -7163,14 +7188,14 @@
       <c r="E18" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>362</v>
       </c>
-      <c r="I18" s="49" t="s">
+      <c r="J18" s="49" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>245</v>
       </c>
@@ -7183,12 +7208,15 @@
       <c r="F19" s="2">
         <v>-1</v>
       </c>
-      <c r="G19" s="23" t="s">
+      <c r="G19" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H19" s="23" t="s">
         <v>345</v>
       </c>
-      <c r="H19" s="23"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I19" s="23"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>246</v>
       </c>
@@ -7201,11 +7229,14 @@
       <c r="F20" s="2">
         <v>-1</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="G20" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H20" s="23" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>221</v>
       </c>
@@ -7218,11 +7249,14 @@
       <c r="F21" s="2">
         <v>-1</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H21" s="23" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>223</v>
       </c>
@@ -7235,11 +7269,14 @@
       <c r="F22" s="2">
         <v>-1</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H22" s="23" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>224</v>
       </c>
@@ -7252,11 +7289,14 @@
       <c r="F23" s="2">
         <v>-1</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H23" s="23" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>226</v>
       </c>
@@ -7269,15 +7309,18 @@
       <c r="F24" s="2">
         <v>-1</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H24" s="23" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="D25" s="37"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>289</v>
       </c>
@@ -7294,14 +7337,14 @@
       <c r="F26" s="2">
         <v>1</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>321</v>
       </c>
-      <c r="I26" s="40" t="s">
+      <c r="J26" s="40" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>290</v>
       </c>
@@ -7318,14 +7361,14 @@
       <c r="F27" s="2">
         <v>2</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>322</v>
       </c>
-      <c r="I27" s="50" t="s">
+      <c r="J27" s="50" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>291</v>
       </c>
@@ -7342,14 +7385,14 @@
       <c r="F28" s="2">
         <v>3</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>323</v>
       </c>
-      <c r="I28" s="51" t="s">
+      <c r="J28" s="51" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>153</v>
       </c>
@@ -7364,11 +7407,11 @@
       <c r="F29" s="2">
         <v>4</v>
       </c>
-      <c r="H29" t="s">
+      <c r="I29" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>282</v>
       </c>
@@ -7385,14 +7428,14 @@
       <c r="F30" s="2">
         <v>5</v>
       </c>
-      <c r="H30" t="s">
+      <c r="I30" t="s">
         <v>288</v>
       </c>
-      <c r="I30" s="40" t="s">
+      <c r="J30" s="40" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="53" t="s">
         <v>325</v>
       </c>
@@ -7409,14 +7452,14 @@
       <c r="F31" s="54">
         <v>6</v>
       </c>
-      <c r="H31" t="s">
+      <c r="I31" t="s">
         <v>360</v>
       </c>
-      <c r="I31" s="55" t="s">
+      <c r="J31" s="55" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="53" t="s">
         <v>326</v>
       </c>
@@ -7433,14 +7476,14 @@
       <c r="F32" s="54">
         <v>7</v>
       </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>361</v>
       </c>
-      <c r="I32" s="23" t="s">
+      <c r="J32" s="23" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>154</v>
       </c>
@@ -7452,14 +7495,17 @@
       <c r="F33" s="2">
         <v>-1</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G33" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H33" t="s">
         <v>567</v>
       </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>155</v>
       </c>
@@ -7471,14 +7517,17 @@
       <c r="F34" s="2">
         <v>-1</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H34" t="s">
         <v>568</v>
       </c>
-      <c r="H34" t="s">
+      <c r="I34" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>182</v>
       </c>
@@ -7490,14 +7539,17 @@
       <c r="F35" s="2">
         <v>-1</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H35" t="s">
         <v>569</v>
       </c>
-      <c r="H35" t="s">
+      <c r="I35" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>183</v>
       </c>
@@ -7509,14 +7561,17 @@
       <c r="F36" s="2">
         <v>-1</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H36" t="s">
         <v>571</v>
       </c>
-      <c r="H36" t="s">
+      <c r="I36" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>184</v>
       </c>
@@ -7528,14 +7583,17 @@
       <c r="F37" s="2">
         <v>-1</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H37" t="s">
         <v>570</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>283</v>
       </c>
@@ -7546,11 +7604,14 @@
       <c r="F38" s="2">
         <v>-1</v>
       </c>
-      <c r="G38" s="35" t="s">
+      <c r="G38" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H38" s="35" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -7563,12 +7624,15 @@
       <c r="F39" s="2">
         <v>-1</v>
       </c>
-      <c r="G39" s="23" t="s">
+      <c r="G39" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H39" s="23" t="s">
         <v>283</v>
       </c>
-      <c r="H39" s="23"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I39" s="23"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -7581,11 +7645,14 @@
       <c r="F40" s="2">
         <v>-1</v>
       </c>
-      <c r="G40" s="23" t="s">
+      <c r="G40" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H40" s="23" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -7598,11 +7665,14 @@
       <c r="F41" s="2">
         <v>-1</v>
       </c>
-      <c r="G41" s="23" t="s">
+      <c r="G41" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H41" s="23" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -7615,15 +7685,18 @@
       <c r="F42" s="2">
         <v>-1</v>
       </c>
-      <c r="G42" s="23" t="s">
+      <c r="G42" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H42" s="23" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B43" s="2"/>
-      <c r="G43"/>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H43"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>274</v>
       </c>
@@ -7640,11 +7713,14 @@
       <c r="F44" s="2">
         <v>2</v>
       </c>
-      <c r="H44" t="s">
+      <c r="G44" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I44" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -7661,16 +7737,19 @@
       <c r="F45" s="2">
         <v>3</v>
       </c>
-      <c r="H45" t="s">
+      <c r="G45" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I45" t="s">
         <v>363</v>
       </c>
-      <c r="I45" s="23"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J45" s="23"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
       <c r="D46"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>156</v>
       </c>
@@ -7690,7 +7769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>185</v>
       </c>
@@ -7710,7 +7789,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>157</v>
       </c>
@@ -7730,7 +7809,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>158</v>
       </c>
@@ -7750,7 +7829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>159</v>
       </c>
@@ -7770,7 +7849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>186</v>
       </c>
@@ -7789,9 +7868,9 @@
       <c r="F52" s="2">
         <v>6</v>
       </c>
-      <c r="I52" s="23"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J52" s="23"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>187</v>
       </c>
@@ -7810,9 +7889,9 @@
       <c r="F53" s="2">
         <v>7</v>
       </c>
-      <c r="I53" s="23"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J53" s="23"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>188</v>
       </c>
@@ -7831,15 +7910,15 @@
       <c r="F54" s="2">
         <v>8</v>
       </c>
-      <c r="I54" s="23"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J54" s="23"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="53"/>
       <c r="D55"/>
-      <c r="I55" s="23"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J55" s="23"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>160</v>
       </c>
@@ -7858,14 +7937,14 @@
       <c r="F56" s="2">
         <v>1</v>
       </c>
-      <c r="H56" t="s">
+      <c r="I56" t="s">
         <v>305</v>
       </c>
-      <c r="I56" s="39" t="s">
+      <c r="J56" s="39" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>161</v>
       </c>
@@ -7884,14 +7963,17 @@
       <c r="F57" s="2">
         <v>2</v>
       </c>
-      <c r="H57" t="s">
+      <c r="G57" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I57" t="s">
         <v>306</v>
       </c>
-      <c r="I57" s="2" t="s">
+      <c r="J57" s="2" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>162</v>
       </c>
@@ -7910,14 +7992,17 @@
       <c r="F58" s="2">
         <v>3</v>
       </c>
-      <c r="H58" t="s">
+      <c r="G58" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I58" t="s">
         <v>307</v>
       </c>
-      <c r="I58" s="39" t="s">
+      <c r="J58" s="39" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>163</v>
       </c>
@@ -7936,14 +8021,17 @@
       <c r="F59" s="2">
         <v>4</v>
       </c>
-      <c r="H59" t="s">
+      <c r="G59" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I59" t="s">
         <v>308</v>
       </c>
-      <c r="I59" s="39" t="s">
+      <c r="J59" s="39" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>165</v>
       </c>
@@ -7962,14 +8050,14 @@
       <c r="F60" s="2">
         <v>5</v>
       </c>
-      <c r="H60" t="s">
+      <c r="I60" t="s">
         <v>305</v>
       </c>
-      <c r="I60" s="39" t="s">
+      <c r="J60" s="39" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>166</v>
       </c>
@@ -7988,14 +8076,17 @@
       <c r="F61" s="2">
         <v>6</v>
       </c>
-      <c r="H61" t="s">
+      <c r="G61" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I61" t="s">
         <v>306</v>
       </c>
-      <c r="I61" s="39" t="s">
+      <c r="J61" s="39" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>167</v>
       </c>
@@ -8014,14 +8105,17 @@
       <c r="F62" s="2">
         <v>7</v>
       </c>
-      <c r="H62" t="s">
+      <c r="G62" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I62" t="s">
         <v>307</v>
       </c>
-      <c r="I62" s="39" t="s">
+      <c r="J62" s="39" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>168</v>
       </c>
@@ -8040,14 +8134,17 @@
       <c r="F63" s="2">
         <v>8</v>
       </c>
-      <c r="H63" t="s">
+      <c r="G63" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I63" t="s">
         <v>308</v>
       </c>
-      <c r="I63" s="39" t="s">
+      <c r="J63" s="39" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>170</v>
       </c>
@@ -8066,14 +8163,14 @@
       <c r="F64" s="39">
         <v>9</v>
       </c>
-      <c r="H64" t="s">
+      <c r="I64" t="s">
         <v>305</v>
       </c>
-      <c r="I64" s="39" t="s">
+      <c r="J64" s="39" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>171</v>
       </c>
@@ -8092,14 +8189,14 @@
       <c r="F65" s="2">
         <v>10</v>
       </c>
-      <c r="H65" t="s">
+      <c r="I65" t="s">
         <v>306</v>
       </c>
-      <c r="I65" s="2" t="s">
+      <c r="J65" s="2" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>172</v>
       </c>
@@ -8118,14 +8215,14 @@
       <c r="F66" s="39">
         <v>11</v>
       </c>
-      <c r="H66" t="s">
+      <c r="I66" t="s">
         <v>307</v>
       </c>
-      <c r="I66" s="2" t="s">
+      <c r="J66" s="2" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>173</v>
       </c>
@@ -8144,14 +8241,14 @@
       <c r="F67" s="2">
         <v>12</v>
       </c>
-      <c r="H67" t="s">
+      <c r="I67" t="s">
         <v>308</v>
       </c>
-      <c r="I67" s="2" t="s">
+      <c r="J67" s="2" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>189</v>
       </c>
@@ -8170,14 +8267,14 @@
       <c r="F68" s="39">
         <v>13</v>
       </c>
-      <c r="H68" t="s">
+      <c r="I68" t="s">
         <v>305</v>
       </c>
-      <c r="I68" s="2" t="s">
+      <c r="J68" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>190</v>
       </c>
@@ -8196,14 +8293,17 @@
       <c r="F69" s="2">
         <v>14</v>
       </c>
-      <c r="H69" t="s">
+      <c r="G69" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I69" t="s">
         <v>306</v>
       </c>
-      <c r="I69" s="2" t="s">
+      <c r="J69" s="2" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>191</v>
       </c>
@@ -8222,14 +8322,17 @@
       <c r="F70" s="39">
         <v>15</v>
       </c>
-      <c r="H70" t="s">
+      <c r="G70" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I70" t="s">
         <v>307</v>
       </c>
-      <c r="I70" s="2" t="s">
+      <c r="J70" s="2" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>192</v>
       </c>
@@ -8248,12 +8351,15 @@
       <c r="F71" s="2">
         <v>16</v>
       </c>
-      <c r="H71" t="s">
+      <c r="G71" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I71" t="s">
         <v>308</v>
       </c>
-      <c r="I71" s="23"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J71" s="23"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>194</v>
       </c>
@@ -8272,14 +8378,14 @@
       <c r="F72" s="39">
         <v>17</v>
       </c>
-      <c r="H72" t="s">
+      <c r="I72" t="s">
         <v>305</v>
       </c>
-      <c r="I72" s="2" t="s">
+      <c r="J72" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>195</v>
       </c>
@@ -8298,14 +8404,17 @@
       <c r="F73" s="2">
         <v>18</v>
       </c>
-      <c r="H73" t="s">
+      <c r="G73" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I73" t="s">
         <v>306</v>
       </c>
-      <c r="I73" s="2" t="s">
+      <c r="J73" s="2" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>196</v>
       </c>
@@ -8324,14 +8433,17 @@
       <c r="F74" s="39">
         <v>19</v>
       </c>
-      <c r="H74" t="s">
+      <c r="G74" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I74" t="s">
         <v>307</v>
       </c>
-      <c r="I74" s="2" t="s">
+      <c r="J74" s="2" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>197</v>
       </c>
@@ -8350,12 +8462,15 @@
       <c r="F75" s="2">
         <v>20</v>
       </c>
-      <c r="H75" t="s">
+      <c r="G75" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I75" t="s">
         <v>308</v>
       </c>
-      <c r="I75" s="23"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J75" s="23"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>199</v>
       </c>
@@ -8374,14 +8489,14 @@
       <c r="F76" s="39">
         <v>21</v>
       </c>
-      <c r="H76" t="s">
+      <c r="I76" t="s">
         <v>305</v>
       </c>
-      <c r="I76" s="2" t="s">
+      <c r="J76" s="2" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>200</v>
       </c>
@@ -8400,14 +8515,14 @@
       <c r="F77" s="2">
         <v>22</v>
       </c>
-      <c r="H77" t="s">
+      <c r="I77" t="s">
         <v>306</v>
       </c>
-      <c r="I77" s="2" t="s">
+      <c r="J77" s="2" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>201</v>
       </c>
@@ -8426,14 +8541,14 @@
       <c r="F78" s="39">
         <v>23</v>
       </c>
-      <c r="H78" t="s">
+      <c r="I78" t="s">
         <v>307</v>
       </c>
-      <c r="I78" s="2" t="s">
+      <c r="J78" s="2" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>202</v>
       </c>
@@ -8452,19 +8567,19 @@
       <c r="F79" s="2">
         <v>24</v>
       </c>
-      <c r="H79" t="s">
+      <c r="I79" t="s">
         <v>308</v>
       </c>
-      <c r="I79" s="2" t="s">
+      <c r="J79" s="2" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B80" s="2"/>
       <c r="D80"/>
-      <c r="I80" s="2"/>
-    </row>
-    <row r="81" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J80" s="2"/>
+    </row>
+    <row r="81" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>351</v>
       </c>
@@ -8483,14 +8598,14 @@
       <c r="F81" s="2">
         <v>1</v>
       </c>
-      <c r="H81" t="s">
+      <c r="I81" t="s">
         <v>347</v>
       </c>
-      <c r="I81" s="56" t="s">
+      <c r="J81" s="56" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>348</v>
       </c>
@@ -8509,17 +8624,17 @@
       <c r="F82" s="2">
         <v>2</v>
       </c>
-      <c r="H82" t="s">
+      <c r="I82" t="s">
         <v>347</v>
       </c>
-      <c r="I82" s="56" t="s">
+      <c r="J82" s="56" t="s">
         <v>502</v>
       </c>
-      <c r="N82" s="55" t="s">
+      <c r="O82" s="55" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>349</v>
       </c>
@@ -8538,14 +8653,14 @@
       <c r="F83" s="41">
         <v>3</v>
       </c>
-      <c r="H83" t="s">
+      <c r="I83" t="s">
         <v>347</v>
       </c>
-      <c r="I83" s="57" t="s">
+      <c r="J83" s="57" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>350</v>
       </c>
@@ -8564,14 +8679,14 @@
       <c r="F84" s="2">
         <v>4</v>
       </c>
-      <c r="H84" t="s">
+      <c r="I84" t="s">
         <v>347</v>
       </c>
-      <c r="I84" s="55" t="s">
+      <c r="J84" s="55" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>353</v>
       </c>
@@ -8590,14 +8705,14 @@
       <c r="F85" s="2">
         <v>5</v>
       </c>
-      <c r="H85" t="s">
+      <c r="I85" t="s">
         <v>347</v>
       </c>
-      <c r="I85" s="55" t="s">
+      <c r="J85" s="55" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>352</v>
       </c>
@@ -8616,14 +8731,14 @@
       <c r="F86" s="2">
         <v>6</v>
       </c>
-      <c r="H86" t="s">
+      <c r="I86" t="s">
         <v>347</v>
       </c>
-      <c r="I86" s="58" t="s">
+      <c r="J86" s="58" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>193</v>
       </c>
@@ -8640,12 +8755,12 @@
       <c r="F87" s="2">
         <v>7</v>
       </c>
-      <c r="H87" t="s">
+      <c r="I87" t="s">
         <v>309</v>
       </c>
-      <c r="I87" s="23"/>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J87" s="23"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>198</v>
       </c>
@@ -8662,12 +8777,12 @@
       <c r="F88" s="2">
         <v>8</v>
       </c>
-      <c r="H88" t="s">
+      <c r="I88" t="s">
         <v>309</v>
       </c>
-      <c r="I88" s="23"/>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J88" s="23"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>164</v>
       </c>
@@ -8684,12 +8799,12 @@
       <c r="F89" s="2">
         <v>9</v>
       </c>
-      <c r="H89" t="s">
+      <c r="I89" t="s">
         <v>309</v>
       </c>
-      <c r="I89" s="23"/>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J89" s="23"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>169</v>
       </c>
@@ -8706,17 +8821,17 @@
       <c r="F90" s="2">
         <v>10</v>
       </c>
-      <c r="H90" t="s">
+      <c r="I90" t="s">
         <v>309</v>
       </c>
-      <c r="I90" s="23"/>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J90" s="23"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B91" s="2"/>
       <c r="D91"/>
-      <c r="I91" s="23"/>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J91" s="23"/>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>519</v>
       </c>
@@ -8735,11 +8850,11 @@
       <c r="F92" s="2">
         <v>1</v>
       </c>
-      <c r="I92" s="45" t="s">
+      <c r="J92" s="45" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>520</v>
       </c>
@@ -8758,11 +8873,11 @@
       <c r="F93" s="2">
         <v>2</v>
       </c>
-      <c r="I93" s="45" t="s">
+      <c r="J93" s="45" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>521</v>
       </c>
@@ -8781,11 +8896,11 @@
       <c r="F94" s="2">
         <v>3</v>
       </c>
-      <c r="I94" s="45" t="s">
+      <c r="J94" s="45" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>516</v>
       </c>
@@ -8804,14 +8919,17 @@
       <c r="F95" s="2">
         <v>4</v>
       </c>
-      <c r="H95" t="s">
+      <c r="G95" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I95" t="s">
         <v>285</v>
       </c>
-      <c r="I95" s="2" t="s">
+      <c r="J95" s="2" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>517</v>
       </c>
@@ -8830,14 +8948,17 @@
       <c r="F96" s="39">
         <v>5</v>
       </c>
-      <c r="H96" t="s">
+      <c r="G96" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I96" t="s">
         <v>285</v>
       </c>
-      <c r="I96" s="2" t="s">
+      <c r="J96" s="2" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>518</v>
       </c>
@@ -8856,14 +8977,14 @@
       <c r="F97" s="2">
         <v>6</v>
       </c>
-      <c r="H97" t="s">
+      <c r="I97" t="s">
         <v>285</v>
       </c>
-      <c r="I97" s="2" t="s">
+      <c r="J97" s="2" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>522</v>
       </c>
@@ -8882,11 +9003,11 @@
       <c r="F98" s="2">
         <v>7</v>
       </c>
-      <c r="I98" s="45" t="s">
+      <c r="J98" s="45" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>523</v>
       </c>
@@ -8905,11 +9026,11 @@
       <c r="F99" s="2">
         <v>8</v>
       </c>
-      <c r="I99" s="45" t="s">
+      <c r="J99" s="45" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>524</v>
       </c>
@@ -8928,11 +9049,11 @@
       <c r="F100" s="2">
         <v>9</v>
       </c>
-      <c r="I100" s="45" t="s">
+      <c r="J100" s="45" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>525</v>
       </c>
@@ -8951,14 +9072,17 @@
       <c r="F101" s="2">
         <v>10</v>
       </c>
-      <c r="H101" t="s">
+      <c r="G101" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I101" t="s">
         <v>285</v>
       </c>
-      <c r="I101" s="2" t="s">
+      <c r="J101" s="2" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>526</v>
       </c>
@@ -8977,14 +9101,17 @@
       <c r="F102" s="39">
         <v>11</v>
       </c>
-      <c r="H102" t="s">
+      <c r="G102" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="I102" t="s">
         <v>285</v>
       </c>
-      <c r="I102" s="2" t="s">
+      <c r="J102" s="2" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>527</v>
       </c>
@@ -9003,37 +9130,32 @@
       <c r="F103" s="2">
         <v>12</v>
       </c>
-      <c r="H103" t="s">
+      <c r="I103" t="s">
         <v>285</v>
       </c>
-      <c r="I103" s="2" t="s">
+      <c r="J103" s="2" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B104" s="2"/>
       <c r="D104"/>
-      <c r="I104" s="2"/>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I105" s="60"/>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I106" s="60"/>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I107" s="61"/>
+      <c r="J104" s="2"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J105" s="60"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J106" s="60"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J107" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9045,22 +9167,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="77" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>269</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added num_vac [Number of people vaccinated] to cascade and databook, to allow quicker equilibration for Pop:0-4
</commit_message>
<xml_diff>
--- a/project/cascade-belarus.xlsx
+++ b/project/cascade-belarus.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-5400" yWindow="-23220" windowWidth="35020" windowHeight="20860" activeTab="3"/>
+    <workbookView xWindow="260" yWindow="-23540" windowWidth="25600" windowHeight="21120" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Sheet Names" sheetId="5" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1205" uniqueCount="579">
   <si>
     <t>Code Label</t>
   </si>
@@ -1987,6 +1987,12 @@
   </si>
   <si>
     <t>Calibrate?</t>
+  </si>
+  <si>
+    <t>num_vac</t>
+  </si>
+  <si>
+    <t>Number of vaccinated people</t>
   </si>
 </sst>
 </file>
@@ -3759,8 +3765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI35"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AJ20" sqref="AJ20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L42" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5472,8 +5478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5546,9 +5552,6 @@
       <c r="D2" s="2">
         <v>-1</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>433</v>
-      </c>
       <c r="J2" t="s">
         <v>206</v>
       </c>
@@ -5581,6 +5584,9 @@
       <c r="D3" s="2">
         <v>3</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>433</v>
+      </c>
       <c r="J3" t="s">
         <v>127</v>
       </c>
@@ -5792,9 +5798,6 @@
       <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>433</v>
-      </c>
       <c r="J11" t="s">
         <v>203</v>
       </c>
@@ -5853,9 +5856,6 @@
       <c r="C13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>433</v>
-      </c>
       <c r="G13" s="2" t="s">
         <v>47</v>
       </c>
@@ -6110,6 +6110,26 @@
         <v>51</v>
       </c>
     </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>577</v>
+      </c>
+      <c r="B23" t="s">
+        <v>578</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J23" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>327</v>
@@ -6298,9 +6318,6 @@
       <c r="D32" s="2">
         <v>3</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>433</v>
-      </c>
       <c r="J32" t="s">
         <v>41</v>
       </c>
@@ -6777,9 +6794,6 @@
       </c>
       <c r="D53" s="2">
         <v>1</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="J53" t="s">
         <v>392</v>
@@ -6797,8 +6811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Major fix to model initialisation
The algorithm for converting characteristic starting values to
compartment starting values is spelled out in model.py.
Basically, if compartment 'a' is not an entry-point; a = 0.
If compartment 'a' is the entry-point of characteristic 'A', including
'a', 'b', 'c', then; a = A - b - c.
If 'A' only includes 'a', then compartment 'a' initialises with the
interpolated value of characteristic 'A'.
If 'A' includes more than 'a', the values of those compartments must
first be 'calculated' before being used.
So, if calculations are ordered, a = A, b = B - a - c, and c = C - a; b
can subtract a but not c until the next loop after c is calculated.
Complicated, but see model.py for more detail.
</commit_message>
<xml_diff>
--- a/project/cascade-belarus.xlsx
+++ b/project/cascade-belarus.xlsx
@@ -24,6 +24,40 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>David Jacob Kedziora</author>
+  </authors>
+  <commentList>
+    <comment ref="A40" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>David Jacob Kedziora:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Below here is NOT finalised. Beware your DOOM.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>David Jacob Kedziora</author>
@@ -3706,7 +3740,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>129</v>
       </c>
@@ -4797,7 +4831,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:35" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>128</v>
       </c>
@@ -5635,17 +5669,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="63.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
@@ -5944,7 +5978,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>625</v>
       </c>
@@ -5961,7 +5995,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>626</v>
       </c>
@@ -5978,7 +6012,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>628</v>
       </c>
@@ -5995,7 +6029,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>627</v>
       </c>
@@ -6012,7 +6046,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>611</v>
       </c>
@@ -6032,7 +6066,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>612</v>
       </c>
@@ -6052,7 +6086,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>613</v>
       </c>
@@ -6072,7 +6106,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>614</v>
       </c>
@@ -6092,7 +6126,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>615</v>
       </c>
@@ -6112,7 +6146,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>616</v>
       </c>
@@ -6132,7 +6166,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>599</v>
       </c>
@@ -6152,7 +6186,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>601</v>
       </c>
@@ -6172,7 +6206,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>603</v>
       </c>
@@ -6192,7 +6226,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>605</v>
       </c>
@@ -6212,7 +6246,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>606</v>
       </c>
@@ -6232,7 +6266,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>607</v>
       </c>
@@ -6252,7 +6286,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>145</v>
       </c>
@@ -6278,7 +6312,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>174</v>
       </c>
@@ -6304,7 +6338,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -6327,8 +6361,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -6360,8 +6393,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>142</v>
       </c>
@@ -6378,7 +6410,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>143</v>
       </c>
@@ -6395,7 +6427,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>144</v>
       </c>
@@ -6412,7 +6444,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>171</v>
       </c>
@@ -6429,7 +6461,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>172</v>
       </c>
@@ -6446,7 +6478,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>173</v>
       </c>
@@ -6463,7 +6495,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>52</v>
       </c>
@@ -6480,7 +6512,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>146</v>
       </c>
@@ -6500,7 +6532,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>147</v>
       </c>
@@ -6520,7 +6552,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>148</v>
       </c>
@@ -6540,7 +6572,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>175</v>
       </c>
@@ -6560,7 +6592,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>176</v>
       </c>
@@ -6581,7 +6613,7 @@
       </c>
       <c r="O52" s="15"/>
     </row>
-    <row r="53" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>177</v>
       </c>
@@ -6601,7 +6633,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>149</v>
       </c>
@@ -6621,7 +6653,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>178</v>
       </c>
@@ -7254,6 +7286,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7261,8 +7295,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9617,9 +9651,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Hotfix to prevalence initialisation
Forgot to include denominator multiplications when fixing
initialisations yesterday. This has been rectified.
Of course, predictable bad things will happen if using a prevalence as a
denominator, as intended.
Also, cascade loading has been updated so that the Plot Value column can
be shunted after the 'includes' section of the characteristics sheet.
My preference is to remove the plot value column altogether and default
to no characteristics being plotted.
</commit_message>
<xml_diff>
--- a/project/cascade-belarus.xlsx
+++ b/project/cascade-belarus.xlsx
@@ -24,40 +24,6 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>David Jacob Kedziora</author>
-  </authors>
-  <commentList>
-    <comment ref="A40" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>David Jacob Kedziora:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Below here is NOT finalised. Beware your DOOM.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>David Jacob Kedziora</author>
@@ -116,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="635">
   <si>
     <t>Code Label</t>
   </si>
@@ -2000,9 +1966,6 @@
     <t>Disaggregation Ratios</t>
   </si>
   <si>
-    <t>Calibrate?</t>
-  </si>
-  <si>
     <t>num_vac</t>
   </si>
   <si>
@@ -2187,6 +2150,9 @@
   </si>
   <si>
     <t>Current SN Extensively Drug-Resistant Infections on Treatment</t>
+  </si>
+  <si>
+    <t>Calibrate</t>
   </si>
 </sst>
 </file>
@@ -2754,7 +2720,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2932,6 +2898,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="112">
@@ -5669,11 +5641,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53:G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5682,16 +5654,16 @@
     <col min="2" max="2" width="63.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="63" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="8.77734375" customWidth="1"/>
     <col min="17" max="18" width="4.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4.33203125" bestFit="1" customWidth="1"/>
@@ -5704,7 +5676,7 @@
     <col min="29" max="29" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5717,573 +5689,662 @@
       <c r="D1" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="62" t="s">
         <v>19</v>
       </c>
       <c r="F1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="15" t="s">
         <v>428</v>
       </c>
-      <c r="G1" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B2" t="s">
+        <v>587</v>
+      </c>
+      <c r="E2" s="63">
+        <v>50</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>591</v>
+      </c>
+      <c r="B4" t="s">
+        <v>592</v>
+      </c>
+      <c r="E4" s="63">
+        <v>100</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>575</v>
+      </c>
+      <c r="B5" t="s">
         <v>588</v>
       </c>
-      <c r="E2" s="2">
-        <v>50</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>592</v>
-      </c>
-      <c r="B4" t="s">
-        <v>593</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="I5" t="s">
+        <v>205</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>576</v>
+      </c>
+      <c r="B6" t="s">
+        <v>589</v>
+      </c>
+      <c r="E6" s="63">
         <v>100</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>576</v>
-      </c>
-      <c r="B5" t="s">
-        <v>589</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="G6" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="I6" t="s">
+        <v>208</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>586</v>
+      </c>
+      <c r="B7" t="s">
+        <v>590</v>
+      </c>
+      <c r="E7" s="63">
+        <v>200</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>577</v>
-      </c>
-      <c r="B6" t="s">
-        <v>590</v>
-      </c>
-      <c r="E6" s="2">
-        <v>100</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="J6" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>587</v>
-      </c>
-      <c r="B7" t="s">
-        <v>591</v>
-      </c>
-      <c r="E7" s="2">
-        <v>200</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>205</v>
+      <c r="I7" t="s">
+        <v>575</v>
       </c>
       <c r="J7" t="s">
         <v>576</v>
       </c>
-      <c r="K7" t="s">
+      <c r="O7" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>581</v>
+      </c>
+      <c r="B8" t="s">
+        <v>582</v>
+      </c>
+      <c r="I8" t="s">
+        <v>204</v>
+      </c>
+      <c r="J8" t="s">
+        <v>575</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>580</v>
+      </c>
+      <c r="B9" t="s">
+        <v>583</v>
+      </c>
+      <c r="E9" s="63">
+        <v>200</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="I9" t="s">
+        <v>207</v>
+      </c>
+      <c r="J9" t="s">
+        <v>576</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>584</v>
+      </c>
+      <c r="B10" t="s">
+        <v>585</v>
+      </c>
+      <c r="E10" s="63">
+        <v>500</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="I10" t="s">
+        <v>581</v>
+      </c>
+      <c r="J10" t="s">
+        <v>580</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>573</v>
+      </c>
+      <c r="B11" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>582</v>
-      </c>
-      <c r="B8" t="s">
-        <v>583</v>
-      </c>
-      <c r="J8" t="s">
-        <v>204</v>
-      </c>
-      <c r="K8" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="I11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J11" t="s">
         <v>581</v>
       </c>
-      <c r="B9" t="s">
-        <v>584</v>
-      </c>
-      <c r="E9" s="2">
-        <v>200</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="J9" t="s">
-        <v>207</v>
-      </c>
-      <c r="K9" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>585</v>
-      </c>
-      <c r="B10" t="s">
-        <v>586</v>
-      </c>
-      <c r="E10" s="2">
-        <v>500</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="J10" t="s">
-        <v>582</v>
-      </c>
-      <c r="K10" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="O11" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>574</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>578</v>
       </c>
-      <c r="J11" t="s">
-        <v>203</v>
-      </c>
-      <c r="K11" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>575</v>
-      </c>
-      <c r="B12" t="s">
-        <v>579</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="E12" s="63">
         <v>400</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>206</v>
       </c>
+      <c r="I12" t="s">
+        <v>206</v>
+      </c>
       <c r="J12" t="s">
-        <v>206</v>
-      </c>
-      <c r="K12" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+        <v>580</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>580</v>
-      </c>
-      <c r="E13" s="2">
+        <v>579</v>
+      </c>
+      <c r="E13" s="63">
         <v>1000</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>203</v>
+      </c>
+      <c r="I13" t="s">
+        <v>573</v>
       </c>
       <c r="J13" t="s">
         <v>574</v>
       </c>
-      <c r="K13" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O13" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>593</v>
+      </c>
+      <c r="B15" t="s">
         <v>594</v>
       </c>
-      <c r="B15" t="s">
-        <v>595</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="E15" s="63">
         <v>30</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="J15" t="s">
+      <c r="I15" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+      <c r="O15" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>622</v>
+      </c>
+      <c r="B16" t="s">
+        <v>628</v>
+      </c>
+      <c r="E16" s="63">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I16" t="s">
+        <v>126</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>623</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>629</v>
       </c>
-      <c r="E16" s="2">
-        <v>10</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="J16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="E17" s="63">
+        <v>20</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17" t="s">
+        <v>129</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>624</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>630</v>
       </c>
-      <c r="E17" s="2">
-        <v>20</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J17" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="E18" s="63">
+        <v>30</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I18" t="s">
+        <v>132</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>625</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>631</v>
       </c>
-      <c r="E18" s="2">
-        <v>30</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="J18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="E19" s="63">
+        <v>40</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="I19" t="s">
+        <v>135</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>627</v>
+      </c>
+      <c r="B20" t="s">
+        <v>632</v>
+      </c>
+      <c r="E20" s="63">
+        <v>50</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="I20" t="s">
+        <v>138</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>626</v>
       </c>
-      <c r="B19" t="s">
-        <v>632</v>
-      </c>
-      <c r="E19" s="2">
-        <v>40</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="J19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>628</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>633</v>
       </c>
-      <c r="E20" s="2">
-        <v>50</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="J20" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="E21" s="63">
+        <v>60</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I21" t="s">
+        <v>141</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>610</v>
+      </c>
+      <c r="B22" t="s">
+        <v>616</v>
+      </c>
+      <c r="E22" s="63">
+        <v>120</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I22" t="s">
+        <v>125</v>
+      </c>
+      <c r="J22" t="s">
+        <v>622</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>611</v>
+      </c>
+      <c r="B23" t="s">
+        <v>617</v>
+      </c>
+      <c r="E23" s="63">
+        <v>110</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I23" t="s">
+        <v>128</v>
+      </c>
+      <c r="J23" t="s">
+        <v>623</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>612</v>
+      </c>
+      <c r="B24" t="s">
+        <v>618</v>
+      </c>
+      <c r="E24" s="63">
+        <v>100</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I24" t="s">
+        <v>131</v>
+      </c>
+      <c r="J24" t="s">
+        <v>624</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>613</v>
+      </c>
+      <c r="B25" t="s">
+        <v>619</v>
+      </c>
+      <c r="E25" s="63">
+        <v>90</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I25" t="s">
+        <v>134</v>
+      </c>
+      <c r="J25" t="s">
+        <v>625</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>614</v>
+      </c>
+      <c r="B26" t="s">
+        <v>620</v>
+      </c>
+      <c r="E26" s="63">
+        <v>80</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I26" t="s">
+        <v>137</v>
+      </c>
+      <c r="J26" t="s">
         <v>627</v>
       </c>
-      <c r="B21" t="s">
-        <v>634</v>
-      </c>
-      <c r="E21" s="2">
-        <v>60</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J21" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="O26" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>615</v>
+      </c>
+      <c r="B27" t="s">
+        <v>621</v>
+      </c>
+      <c r="E27" s="63">
+        <v>70</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I27" t="s">
+        <v>140</v>
+      </c>
+      <c r="J27" t="s">
+        <v>626</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>598</v>
+      </c>
+      <c r="B28" t="s">
+        <v>599</v>
+      </c>
+      <c r="E28" s="63">
+        <v>130</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="I28" t="s">
+        <v>124</v>
+      </c>
+      <c r="J28" t="s">
+        <v>610</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>600</v>
+      </c>
+      <c r="B29" t="s">
+        <v>601</v>
+      </c>
+      <c r="E29" s="63">
+        <v>140</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I29" t="s">
+        <v>127</v>
+      </c>
+      <c r="J29" t="s">
         <v>611</v>
       </c>
-      <c r="B22" t="s">
-        <v>617</v>
-      </c>
-      <c r="E22" s="2">
-        <v>120</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="J22" t="s">
-        <v>125</v>
-      </c>
-      <c r="K22" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="O29" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>602</v>
+      </c>
+      <c r="B30" t="s">
+        <v>603</v>
+      </c>
+      <c r="E30" s="63">
+        <v>150</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="I30" t="s">
+        <v>130</v>
+      </c>
+      <c r="J30" t="s">
         <v>612</v>
       </c>
-      <c r="B23" t="s">
-        <v>618</v>
-      </c>
-      <c r="E23" s="2">
-        <v>110</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="J23" t="s">
-        <v>128</v>
-      </c>
-      <c r="K23" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="O30" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>604</v>
+      </c>
+      <c r="B31" t="s">
+        <v>607</v>
+      </c>
+      <c r="E31" s="63">
+        <v>160</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I31" t="s">
+        <v>133</v>
+      </c>
+      <c r="J31" t="s">
         <v>613</v>
       </c>
-      <c r="B24" t="s">
-        <v>619</v>
-      </c>
-      <c r="E24" s="2">
-        <v>100</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="J24" t="s">
-        <v>131</v>
-      </c>
-      <c r="K24" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="O31" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>605</v>
+      </c>
+      <c r="B32" t="s">
+        <v>608</v>
+      </c>
+      <c r="E32" s="63">
+        <v>170</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I32" t="s">
+        <v>136</v>
+      </c>
+      <c r="J32" t="s">
         <v>614</v>
       </c>
-      <c r="B25" t="s">
-        <v>620</v>
-      </c>
-      <c r="E25" s="2">
-        <v>90</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J25" t="s">
-        <v>134</v>
-      </c>
-      <c r="K25" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>615</v>
-      </c>
-      <c r="B26" t="s">
-        <v>621</v>
-      </c>
-      <c r="E26" s="2">
-        <v>80</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="J26" t="s">
-        <v>137</v>
-      </c>
-      <c r="K26" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>616</v>
-      </c>
-      <c r="B27" t="s">
-        <v>622</v>
-      </c>
-      <c r="E27" s="2">
-        <v>70</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="J27" t="s">
-        <v>140</v>
-      </c>
-      <c r="K27" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>599</v>
-      </c>
-      <c r="B28" t="s">
-        <v>600</v>
-      </c>
-      <c r="E28" s="2">
-        <v>130</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="J28" t="s">
-        <v>124</v>
-      </c>
-      <c r="K28" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>601</v>
-      </c>
-      <c r="B29" t="s">
-        <v>602</v>
-      </c>
-      <c r="E29" s="2">
-        <v>140</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="J29" t="s">
-        <v>127</v>
-      </c>
-      <c r="K29" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>603</v>
-      </c>
-      <c r="B30" t="s">
-        <v>604</v>
-      </c>
-      <c r="E30" s="2">
-        <v>150</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="J30" t="s">
-        <v>130</v>
-      </c>
-      <c r="K30" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>605</v>
-      </c>
-      <c r="B31" t="s">
-        <v>608</v>
-      </c>
-      <c r="E31" s="2">
-        <v>160</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J31" t="s">
-        <v>133</v>
-      </c>
-      <c r="K31" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>606</v>
-      </c>
-      <c r="B32" t="s">
-        <v>609</v>
-      </c>
-      <c r="E32" s="2">
-        <v>170</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="J32" t="s">
-        <v>136</v>
-      </c>
-      <c r="K32" t="s">
-        <v>615</v>
+      <c r="O32" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B33" t="s">
-        <v>610</v>
-      </c>
-      <c r="E33" s="2">
+        <v>609</v>
+      </c>
+      <c r="E33" s="63">
         <v>180</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="I33" t="s">
+        <v>139</v>
+      </c>
       <c r="J33" t="s">
-        <v>139</v>
-      </c>
-      <c r="K33" t="s">
-        <v>616</v>
+        <v>615</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -6291,25 +6352,28 @@
         <v>145</v>
       </c>
       <c r="B34" t="s">
+        <v>597</v>
+      </c>
+      <c r="E34" s="63">
+        <v>500</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="I34" t="s">
+        <v>201</v>
+      </c>
+      <c r="J34" t="s">
         <v>598</v>
       </c>
-      <c r="E34" s="2">
-        <v>500</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="J34" t="s">
-        <v>201</v>
-      </c>
       <c r="K34" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="L34" t="s">
-        <v>601</v>
-      </c>
-      <c r="M34" t="s">
-        <v>603</v>
+        <v>602</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
@@ -6317,16 +6381,19 @@
         <v>174</v>
       </c>
       <c r="B35" t="s">
-        <v>597</v>
-      </c>
-      <c r="E35" s="2">
+        <v>596</v>
+      </c>
+      <c r="E35" s="63">
         <v>600</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>202</v>
       </c>
+      <c r="I35" t="s">
+        <v>202</v>
+      </c>
       <c r="J35" t="s">
-        <v>202</v>
+        <v>604</v>
       </c>
       <c r="K35" t="s">
         <v>605</v>
@@ -6334,8 +6401,8 @@
       <c r="L35" t="s">
         <v>606</v>
       </c>
-      <c r="M35" t="s">
-        <v>607</v>
+      <c r="O35" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
@@ -6343,22 +6410,25 @@
         <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>596</v>
-      </c>
-      <c r="E36" s="2">
+        <v>595</v>
+      </c>
+      <c r="E36" s="63">
         <v>1200</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>200</v>
       </c>
+      <c r="I36" t="s">
+        <v>200</v>
+      </c>
       <c r="J36" t="s">
-        <v>200</v>
+        <v>145</v>
       </c>
       <c r="K36" t="s">
-        <v>145</v>
-      </c>
-      <c r="L36" t="s">
         <v>174</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
@@ -6368,29 +6438,32 @@
       <c r="B38" t="s">
         <v>59</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="63">
         <v>3000</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="I38" t="s">
+        <v>2</v>
+      </c>
       <c r="J38" t="s">
-        <v>2</v>
+        <v>572</v>
       </c>
       <c r="K38" t="s">
-        <v>573</v>
+        <v>591</v>
       </c>
       <c r="L38" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="M38" t="s">
-        <v>594</v>
+        <v>49</v>
       </c>
       <c r="N38" t="s">
-        <v>49</v>
-      </c>
-      <c r="O38" t="s">
         <v>50</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
@@ -6400,14 +6473,14 @@
       <c r="B40" t="s">
         <v>84</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>429</v>
+      <c r="I40" t="s">
+        <v>124</v>
       </c>
       <c r="J40" t="s">
-        <v>124</v>
-      </c>
-      <c r="K40" t="s">
         <v>125</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
@@ -6417,14 +6490,14 @@
       <c r="B41" t="s">
         <v>85</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>429</v>
+      <c r="I41" t="s">
+        <v>127</v>
       </c>
       <c r="J41" t="s">
-        <v>127</v>
-      </c>
-      <c r="K41" t="s">
         <v>128</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
@@ -6434,14 +6507,14 @@
       <c r="B42" t="s">
         <v>86</v>
       </c>
-      <c r="F42" s="2" t="s">
-        <v>429</v>
+      <c r="I42" t="s">
+        <v>130</v>
       </c>
       <c r="J42" t="s">
-        <v>130</v>
-      </c>
-      <c r="K42" t="s">
         <v>131</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -6451,14 +6524,14 @@
       <c r="B43" t="s">
         <v>102</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>429</v>
+      <c r="I43" t="s">
+        <v>133</v>
       </c>
       <c r="J43" t="s">
-        <v>133</v>
-      </c>
-      <c r="K43" t="s">
         <v>134</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
@@ -6468,14 +6541,14 @@
       <c r="B44" t="s">
         <v>103</v>
       </c>
-      <c r="F44" s="2" t="s">
-        <v>429</v>
+      <c r="I44" t="s">
+        <v>136</v>
       </c>
       <c r="J44" t="s">
-        <v>136</v>
-      </c>
-      <c r="K44" t="s">
         <v>137</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
@@ -6485,152 +6558,152 @@
       <c r="B45" t="s">
         <v>104</v>
       </c>
-      <c r="F45" s="2" t="s">
-        <v>429</v>
+      <c r="I45" t="s">
+        <v>139</v>
       </c>
       <c r="J45" t="s">
-        <v>139</v>
-      </c>
-      <c r="K45" t="s">
         <v>140</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>146</v>
+      </c>
+      <c r="B46" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H46" t="s">
+        <v>51</v>
+      </c>
+      <c r="I46" t="s">
+        <v>142</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>147</v>
       </c>
       <c r="B47" t="s">
-        <v>60</v>
-      </c>
-      <c r="G47" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H47" t="s">
+        <v>51</v>
+      </c>
       <c r="I47" t="s">
-        <v>51</v>
-      </c>
-      <c r="J47" t="s">
-        <v>49</v>
+        <v>143</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B48" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G48" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H48" t="s">
+        <v>51</v>
+      </c>
       <c r="I48" t="s">
-        <v>51</v>
-      </c>
-      <c r="J48" t="s">
-        <v>142</v>
+        <v>144</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="B49" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G49" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H49" t="s">
+        <v>51</v>
+      </c>
       <c r="I49" t="s">
-        <v>51</v>
-      </c>
-      <c r="J49" t="s">
-        <v>143</v>
+        <v>171</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="B50" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G50" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H50" t="s">
+        <v>51</v>
+      </c>
       <c r="I50" t="s">
-        <v>51</v>
-      </c>
-      <c r="J50" t="s">
-        <v>144</v>
+        <v>172</v>
+      </c>
+      <c r="N50" s="15"/>
+      <c r="O50" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B51" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G51" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H51" t="s">
+        <v>51</v>
+      </c>
       <c r="I51" t="s">
-        <v>51</v>
-      </c>
-      <c r="J51" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>176</v>
-      </c>
-      <c r="B52" t="s">
-        <v>106</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I52" t="s">
-        <v>51</v>
-      </c>
-      <c r="J52" t="s">
-        <v>172</v>
-      </c>
-      <c r="O52" s="15"/>
+        <v>173</v>
+      </c>
+      <c r="O51" s="2" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>177</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G53" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H53" t="s">
+        <v>51</v>
+      </c>
       <c r="I53" t="s">
-        <v>51</v>
-      </c>
-      <c r="J53" t="s">
-        <v>173</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.3">
@@ -6641,16 +6714,16 @@
         <v>120</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G54" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H54" t="s">
+        <v>51</v>
+      </c>
       <c r="I54" t="s">
-        <v>51</v>
-      </c>
-      <c r="J54" t="s">
         <v>145</v>
+      </c>
+      <c r="O54" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
@@ -6661,16 +6734,16 @@
         <v>121</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G55" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H55" t="s">
+        <v>51</v>
+      </c>
       <c r="I55" t="s">
-        <v>51</v>
-      </c>
-      <c r="J55" t="s">
         <v>174</v>
+      </c>
+      <c r="O55" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
@@ -6680,14 +6753,17 @@
       <c r="B56" t="s">
         <v>61</v>
       </c>
-      <c r="G56" s="2" t="s">
+      <c r="F56" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H56" t="s">
+        <v>51</v>
+      </c>
       <c r="I56" t="s">
-        <v>51</v>
-      </c>
-      <c r="J56" t="s">
         <v>50</v>
+      </c>
+      <c r="O56" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
@@ -6697,14 +6773,14 @@
       <c r="B58" t="s">
         <v>337</v>
       </c>
-      <c r="F58" s="2" t="s">
-        <v>429</v>
+      <c r="I58" t="s">
+        <v>205</v>
       </c>
       <c r="J58" t="s">
-        <v>205</v>
-      </c>
-      <c r="K58" t="s">
         <v>208</v>
+      </c>
+      <c r="O58" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
@@ -6714,17 +6790,17 @@
       <c r="B59" t="s">
         <v>336</v>
       </c>
-      <c r="F59" s="2" t="s">
-        <v>429</v>
+      <c r="I59" t="s">
+        <v>126</v>
       </c>
       <c r="J59" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="K59" t="s">
-        <v>129</v>
-      </c>
-      <c r="L59" t="s">
         <v>132</v>
+      </c>
+      <c r="O59" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
@@ -6734,17 +6810,17 @@
       <c r="B60" t="s">
         <v>335</v>
       </c>
-      <c r="F60" s="2" t="s">
-        <v>429</v>
+      <c r="I60" t="s">
+        <v>135</v>
       </c>
       <c r="J60" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="K60" t="s">
-        <v>138</v>
-      </c>
-      <c r="L60" t="s">
         <v>141</v>
+      </c>
+      <c r="O60" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
@@ -6754,14 +6830,14 @@
       <c r="B61" t="s">
         <v>339</v>
       </c>
-      <c r="F61" s="2" t="s">
-        <v>429</v>
+      <c r="I61" t="s">
+        <v>328</v>
       </c>
       <c r="J61" t="s">
-        <v>328</v>
-      </c>
-      <c r="K61" t="s">
         <v>329</v>
+      </c>
+      <c r="O61" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
@@ -6771,14 +6847,14 @@
       <c r="B62" t="s">
         <v>338</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>429</v>
+      <c r="I62" t="s">
+        <v>324</v>
       </c>
       <c r="J62" t="s">
-        <v>324</v>
-      </c>
-      <c r="K62" t="s">
         <v>325</v>
+      </c>
+      <c r="O62" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
@@ -6792,16 +6868,16 @@
         <v>535</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G63" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H63" t="s">
+        <v>51</v>
+      </c>
       <c r="I63" t="s">
-        <v>51</v>
-      </c>
-      <c r="J63" t="s">
         <v>324</v>
+      </c>
+      <c r="O63" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
@@ -6815,19 +6891,19 @@
         <v>535</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G64" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H64" t="s">
+        <v>51</v>
+      </c>
       <c r="I64" t="s">
-        <v>51</v>
-      </c>
-      <c r="J64" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O64" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>331</v>
       </c>
@@ -6838,19 +6914,19 @@
         <v>535</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G65" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H65" t="s">
+        <v>51</v>
+      </c>
       <c r="I65" t="s">
-        <v>51</v>
-      </c>
-      <c r="J65" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O65" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>362</v>
       </c>
@@ -6860,11 +6936,14 @@
       <c r="C66" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="J66" t="s">
+      <c r="I66" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O66" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>372</v>
       </c>
@@ -6875,19 +6954,19 @@
         <v>274</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G67" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H67" t="s">
+        <v>41</v>
+      </c>
       <c r="I67" t="s">
-        <v>41</v>
-      </c>
-      <c r="J67" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O67" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>373</v>
       </c>
@@ -6898,19 +6977,19 @@
         <v>274</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G68" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H68" t="s">
+        <v>41</v>
+      </c>
       <c r="I68" t="s">
-        <v>41</v>
-      </c>
-      <c r="J68" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O68" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>374</v>
       </c>
@@ -6921,19 +7000,19 @@
         <v>274</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G69" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H69" t="s">
+        <v>41</v>
+      </c>
       <c r="I69" t="s">
-        <v>41</v>
-      </c>
-      <c r="J69" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O69" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>369</v>
       </c>
@@ -6944,19 +7023,19 @@
         <v>274</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G70" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H70" t="s">
+        <v>41</v>
+      </c>
       <c r="I70" t="s">
-        <v>41</v>
-      </c>
-      <c r="J70" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O70" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>370</v>
       </c>
@@ -6967,19 +7046,19 @@
         <v>274</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G71" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H71" t="s">
+        <v>41</v>
+      </c>
       <c r="I71" t="s">
-        <v>41</v>
-      </c>
-      <c r="J71" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O71" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>371</v>
       </c>
@@ -6990,19 +7069,19 @@
         <v>274</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="G72" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="H72" t="s">
+        <v>41</v>
+      </c>
       <c r="I72" t="s">
-        <v>41</v>
-      </c>
-      <c r="J72" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O72" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>364</v>
       </c>
@@ -7012,20 +7091,20 @@
       <c r="C73" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F73" s="2" t="s">
-        <v>429</v>
+      <c r="H73" t="s">
+        <v>41</v>
       </c>
       <c r="I73" t="s">
-        <v>41</v>
+        <v>142</v>
       </c>
       <c r="J73" t="s">
-        <v>142</v>
-      </c>
-      <c r="K73" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O73" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>363</v>
       </c>
@@ -7035,20 +7114,20 @@
       <c r="C74" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F74" s="2" t="s">
-        <v>429</v>
+      <c r="H74" t="s">
+        <v>41</v>
       </c>
       <c r="I74" t="s">
-        <v>41</v>
+        <v>143</v>
       </c>
       <c r="J74" t="s">
-        <v>143</v>
-      </c>
-      <c r="K74" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O74" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>365</v>
       </c>
@@ -7058,68 +7137,68 @@
       <c r="C75" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>429</v>
+      <c r="H75" t="s">
+        <v>41</v>
       </c>
       <c r="I75" t="s">
-        <v>41</v>
+        <v>144</v>
       </c>
       <c r="J75" t="s">
-        <v>144</v>
-      </c>
-      <c r="K75" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O75" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>378</v>
       </c>
       <c r="B76" t="s">
         <v>375</v>
       </c>
-      <c r="F76" s="2" t="s">
-        <v>429</v>
+      <c r="I76" t="s">
+        <v>205</v>
       </c>
       <c r="J76" t="s">
-        <v>205</v>
-      </c>
-      <c r="K76" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O76" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>379</v>
       </c>
       <c r="B77" t="s">
         <v>376</v>
       </c>
-      <c r="F77" s="2" t="s">
-        <v>429</v>
+      <c r="I77" t="s">
+        <v>204</v>
       </c>
       <c r="J77" t="s">
-        <v>204</v>
-      </c>
-      <c r="K77" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O77" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>380</v>
       </c>
       <c r="B78" t="s">
         <v>377</v>
       </c>
-      <c r="F78" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="J78" t="s">
+      <c r="I78" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O78" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>381</v>
       </c>
@@ -7129,14 +7208,14 @@
       <c r="C79" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F79" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="J79" t="s">
+      <c r="I79" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="O79" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>382</v>
       </c>
@@ -7146,14 +7225,14 @@
       <c r="C80" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F80" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="J80" t="s">
+      <c r="I80" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O80" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>383</v>
       </c>
@@ -7163,14 +7242,14 @@
       <c r="C81" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F81" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="J81" t="s">
+      <c r="I81" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O81" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>384</v>
       </c>
@@ -7180,14 +7259,14 @@
       <c r="C82" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F82" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="J82" t="s">
+      <c r="I82" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O82" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>385</v>
       </c>
@@ -7197,14 +7276,14 @@
       <c r="C83" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F83" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="J83" t="s">
+      <c r="I83" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O83" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>386</v>
       </c>
@@ -7214,14 +7293,14 @@
       <c r="C84" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F84" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="J84" t="s">
+      <c r="I84" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O84" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>387</v>
       </c>
@@ -7231,20 +7310,20 @@
       <c r="C85" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F85" s="2" t="s">
-        <v>429</v>
+      <c r="I85" t="s">
+        <v>125</v>
       </c>
       <c r="J85" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="K85" t="s">
-        <v>128</v>
-      </c>
-      <c r="L85" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O85" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>388</v>
       </c>
@@ -7254,20 +7333,20 @@
       <c r="C86" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="F86" s="2" t="s">
-        <v>429</v>
+      <c r="I86" t="s">
+        <v>134</v>
       </c>
       <c r="J86" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="K86" t="s">
-        <v>137</v>
-      </c>
-      <c r="L86" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O86" s="2" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>389</v>
       </c>
@@ -7277,17 +7356,19 @@
       <c r="C87" s="2" t="s">
         <v>273</v>
       </c>
+      <c r="I87" t="s">
+        <v>388</v>
+      </c>
       <c r="J87" t="s">
-        <v>388</v>
-      </c>
-      <c r="K87" t="s">
         <v>387</v>
+      </c>
+      <c r="O87" s="2" t="s">
+        <v>429</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7295,8 +7376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:D28"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7334,7 +7415,7 @@
         <v>62</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>572</v>
+        <v>634</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>123</v>
@@ -7933,7 +8014,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="53" t="s">
         <v>322</v>
       </c>
@@ -7957,7 +8038,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="53" t="s">
         <v>323</v>
       </c>
@@ -7981,7 +8062,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>151</v>
       </c>
@@ -8003,7 +8084,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>152</v>
       </c>
@@ -8025,7 +8106,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>179</v>
       </c>
@@ -8047,7 +8128,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>180</v>
       </c>
@@ -8069,7 +8150,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>181</v>
       </c>
@@ -8091,7 +8172,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>280</v>
       </c>
@@ -8109,7 +8190,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -8130,7 +8211,7 @@
       </c>
       <c r="I39" s="23"/>
     </row>
-    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -8150,7 +8231,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -8170,7 +8251,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -8190,11 +8271,11 @@
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="H43"/>
     </row>
-    <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>271</v>
       </c>
@@ -8218,7 +8299,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -8243,11 +8324,11 @@
       </c>
       <c r="J45" s="23"/>
     </row>
-    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
       <c r="D46"/>
     </row>
-    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>153</v>
       </c>
@@ -8267,7 +8348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>182</v>
       </c>
@@ -8287,7 +8368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>154</v>
       </c>
@@ -8307,7 +8388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>155</v>
       </c>
@@ -8327,7 +8408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>156</v>
       </c>
@@ -8347,7 +8428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>183</v>
       </c>
@@ -8368,7 +8449,7 @@
       </c>
       <c r="J52" s="23"/>
     </row>
-    <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>184</v>
       </c>
@@ -8389,7 +8470,7 @@
       </c>
       <c r="J53" s="23"/>
     </row>
-    <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>185</v>
       </c>
@@ -8410,13 +8491,13 @@
       </c>
       <c r="J54" s="23"/>
     </row>
-    <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B55" s="2"/>
       <c r="C55" s="53"/>
       <c r="D55"/>
       <c r="J55" s="23"/>
     </row>
-    <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>157</v>
       </c>
@@ -8442,7 +8523,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>158</v>
       </c>
@@ -8471,7 +8552,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>159</v>
       </c>
@@ -8500,7 +8581,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>160</v>
       </c>
@@ -8529,7 +8610,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>162</v>
       </c>
@@ -8555,7 +8636,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>163</v>
       </c>
@@ -8584,7 +8665,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>164</v>
       </c>
@@ -8613,7 +8694,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>165</v>
       </c>
@@ -8642,7 +8723,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>167</v>
       </c>
@@ -8668,7 +8749,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>168</v>
       </c>
@@ -8694,7 +8775,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>169</v>
       </c>
@@ -8720,7 +8801,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>170</v>
       </c>
@@ -8746,7 +8827,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>186</v>
       </c>
@@ -8772,7 +8853,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>187</v>
       </c>
@@ -8801,7 +8882,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>188</v>
       </c>
@@ -8830,7 +8911,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>189</v>
       </c>
@@ -8857,7 +8938,7 @@
       </c>
       <c r="J71" s="23"/>
     </row>
-    <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>191</v>
       </c>
@@ -8883,7 +8964,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>192</v>
       </c>
@@ -8912,7 +8993,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>193</v>
       </c>
@@ -8941,7 +9022,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>194</v>
       </c>
@@ -8968,7 +9049,7 @@
       </c>
       <c r="J75" s="23"/>
     </row>
-    <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>196</v>
       </c>
@@ -8994,7 +9075,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>197</v>
       </c>
@@ -9020,7 +9101,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>198</v>
       </c>
@@ -9046,7 +9127,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>199</v>
       </c>
@@ -9072,12 +9153,12 @@
         <v>410</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B80" s="2"/>
       <c r="D80"/>
       <c r="J80" s="2"/>
     </row>
-    <row r="81" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>348</v>
       </c>
@@ -9103,7 +9184,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="45" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>345</v>
       </c>
@@ -9132,7 +9213,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>346</v>
       </c>
@@ -9158,7 +9239,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>347</v>
       </c>
@@ -9184,7 +9265,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>350</v>
       </c>
@@ -9210,7 +9291,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>349</v>
       </c>
@@ -9236,7 +9317,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>190</v>
       </c>
@@ -9258,7 +9339,7 @@
       </c>
       <c r="J87" s="23"/>
     </row>
-    <row r="88" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>195</v>
       </c>
@@ -9280,7 +9361,7 @@
       </c>
       <c r="J88" s="23"/>
     </row>
-    <row r="89" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>161</v>
       </c>
@@ -9302,7 +9383,7 @@
       </c>
       <c r="J89" s="23"/>
     </row>
-    <row r="90" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>166</v>
       </c>
@@ -9324,12 +9405,12 @@
       </c>
       <c r="J90" s="23"/>
     </row>
-    <row r="91" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B91" s="2"/>
       <c r="D91"/>
       <c r="J91" s="23"/>
     </row>
-    <row r="92" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>515</v>
       </c>
@@ -9352,7 +9433,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>516</v>
       </c>
@@ -9375,7 +9456,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>517</v>
       </c>
@@ -9398,7 +9479,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>512</v>
       </c>
@@ -9427,7 +9508,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>513</v>
       </c>
@@ -9456,7 +9537,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>514</v>
       </c>
@@ -9482,7 +9563,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>518</v>
       </c>
@@ -9505,7 +9586,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>519</v>
       </c>
@@ -9528,7 +9609,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>520</v>
       </c>
@@ -9551,7 +9632,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>521</v>
       </c>
@@ -9580,7 +9661,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>522</v>
       </c>
@@ -9609,7 +9690,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>523</v>
       </c>
@@ -9635,18 +9716,18 @@
         <v>409</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B104" s="2"/>
       <c r="D104"/>
       <c r="J104" s="2"/>
     </row>
-    <row r="105" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J105" s="60"/>
     </row>
-    <row r="106" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J106" s="60"/>
     </row>
-    <row r="107" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J107" s="61"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Found source of bug for why Optima-TB kept on complaining that a compartment had to be resized: discovered that this was a flow into d_oth (non-TB related deaths). Digging a bit deeper, this was the link from births to d_oth - which we don't need to have! (and doesn't make sense). Updated the cascade spreadsheet to be correct
</commit_message>
<xml_diff>
--- a/project/cascade-belarus.xlsx
+++ b/project/cascade-belarus.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27417"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjarvis/git/tb-ucl/project/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="647" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="-2900" yWindow="-18760" windowWidth="30100" windowHeight="18500" tabRatio="647" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Sheet Names" sheetId="5" r:id="rId1"/>
@@ -16,6 +21,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1340" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="634">
   <si>
     <t>Code Label</t>
   </si>
@@ -2242,7 +2250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2279,6 +2287,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2677,7 +2691,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2833,6 +2847,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3310,13 +3327,13 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>75</v>
       </c>
@@ -3324,7 +3341,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>77</v>
       </c>
@@ -3332,7 +3349,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>548</v>
       </c>
@@ -3340,7 +3357,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>547</v>
       </c>
@@ -3348,7 +3365,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>253</v>
       </c>
@@ -3356,7 +3373,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>452</v>
       </c>
@@ -3364,7 +3381,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>432</v>
       </c>
@@ -3372,7 +3389,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>466</v>
       </c>
@@ -3380,7 +3397,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>431</v>
       </c>
@@ -3388,7 +3405,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>467</v>
       </c>
@@ -3396,7 +3413,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>449</v>
       </c>
@@ -3406,11 +3423,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3422,7 +3434,7 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.83203125" bestFit="1" customWidth="1"/>
@@ -3432,7 +3444,7 @@
     <col min="6" max="7" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3455,7 +3467,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3466,7 +3478,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3477,7 +3489,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>183</v>
       </c>
@@ -3488,7 +3500,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>184</v>
       </c>
@@ -3499,7 +3511,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>185</v>
       </c>
@@ -3510,7 +3522,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>186</v>
       </c>
@@ -3521,7 +3533,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>187</v>
       </c>
@@ -3532,7 +3544,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>188</v>
       </c>
@@ -3543,7 +3555,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>71</v>
       </c>
@@ -3554,7 +3566,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>180</v>
       </c>
@@ -3568,7 +3580,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>181</v>
       </c>
@@ -3582,7 +3594,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>104</v>
       </c>
@@ -3593,7 +3605,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -3604,7 +3616,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>106</v>
       </c>
@@ -3615,7 +3627,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>107</v>
       </c>
@@ -3626,7 +3638,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>108</v>
       </c>
@@ -3637,7 +3649,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>109</v>
       </c>
@@ -3648,7 +3660,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>110</v>
       </c>
@@ -3659,7 +3671,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>111</v>
       </c>
@@ -3670,7 +3682,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>112</v>
       </c>
@@ -3681,7 +3693,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>182</v>
       </c>
@@ -3695,7 +3707,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>113</v>
       </c>
@@ -3706,7 +3718,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>114</v>
       </c>
@@ -3717,7 +3729,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>115</v>
       </c>
@@ -3728,7 +3740,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>116</v>
       </c>
@@ -3739,7 +3751,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>117</v>
       </c>
@@ -3750,7 +3762,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>118</v>
       </c>
@@ -3761,7 +3773,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>119</v>
       </c>
@@ -3772,7 +3784,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>120</v>
       </c>
@@ -3783,7 +3795,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>121</v>
       </c>
@@ -3794,7 +3806,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>72</v>
       </c>
@@ -3805,7 +3817,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -3819,7 +3831,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -3833,7 +3845,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>247</v>
       </c>
@@ -3849,11 +3861,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3861,11 +3868,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AJ4" sqref="AJ4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="2" max="2" width="3.33203125" bestFit="1" customWidth="1"/>
@@ -3902,7 +3909,7 @@
     <col min="35" max="35" width="4.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>247</v>
@@ -4007,7 +4014,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>247</v>
       </c>
@@ -4046,11 +4053,9 @@
       <c r="AF2" s="7"/>
       <c r="AG2" s="6"/>
       <c r="AH2" s="7"/>
-      <c r="AI2" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35">
+      <c r="AI2" s="55"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -4095,7 +4100,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -4138,7 +4143,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>183</v>
       </c>
@@ -4185,7 +4190,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>184</v>
       </c>
@@ -4232,7 +4237,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>185</v>
       </c>
@@ -4277,7 +4282,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
         <v>186</v>
       </c>
@@ -4322,7 +4327,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>187</v>
       </c>
@@ -4367,7 +4372,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
         <v>188</v>
       </c>
@@ -4412,7 +4417,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>71</v>
       </c>
@@ -4455,7 +4460,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>180</v>
       </c>
@@ -4498,7 +4503,7 @@
       <c r="AH12" s="20"/>
       <c r="AI12" s="22"/>
     </row>
-    <row r="13" spans="1:35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>181</v>
       </c>
@@ -4543,7 +4548,7 @@
       <c r="AH13" s="10"/>
       <c r="AI13" s="11"/>
     </row>
-    <row r="14" spans="1:35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>104</v>
       </c>
@@ -4590,7 +4595,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>105</v>
       </c>
@@ -4637,7 +4642,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>106</v>
       </c>
@@ -4686,7 +4691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>107</v>
       </c>
@@ -4733,7 +4738,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>108</v>
       </c>
@@ -4780,7 +4785,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>109</v>
       </c>
@@ -4829,7 +4834,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>110</v>
       </c>
@@ -4876,7 +4881,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>111</v>
       </c>
@@ -4923,7 +4928,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>112</v>
       </c>
@@ -4970,7 +4975,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>182</v>
       </c>
@@ -5015,7 +5020,7 @@
       <c r="AH23" s="7"/>
       <c r="AI23" s="8"/>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>113</v>
       </c>
@@ -5062,7 +5067,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>114</v>
       </c>
@@ -5109,7 +5114,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>115</v>
       </c>
@@ -5158,7 +5163,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>116</v>
       </c>
@@ -5205,7 +5210,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>117</v>
       </c>
@@ -5252,7 +5257,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>118</v>
       </c>
@@ -5301,7 +5306,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>119</v>
       </c>
@@ -5348,7 +5353,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>120</v>
       </c>
@@ -5395,7 +5400,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>121</v>
       </c>
@@ -5442,7 +5447,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>72</v>
       </c>
@@ -5485,7 +5490,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>41</v>
       </c>
@@ -5524,7 +5529,7 @@
       <c r="AH34" s="10"/>
       <c r="AI34" s="11"/>
     </row>
-    <row r="35" spans="1:35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>42</v>
       </c>
@@ -5566,11 +5571,6 @@
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5582,7 +5582,7 @@
       <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.1640625" bestFit="1" customWidth="1"/>
@@ -5610,7 +5610,7 @@
     <col min="29" max="29" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5642,7 +5642,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>468</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>487</v>
       </c>
@@ -5688,7 +5688,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>471</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>472</v>
       </c>
@@ -5731,7 +5731,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>482</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>477</v>
       </c>
@@ -5780,7 +5780,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>476</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>480</v>
       </c>
@@ -5832,7 +5832,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>469</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>470</v>
       </c>
@@ -5881,7 +5881,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>489</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>518</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>519</v>
       </c>
@@ -5976,7 +5976,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>520</v>
       </c>
@@ -5999,7 +5999,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>521</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>523</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>522</v>
       </c>
@@ -6068,7 +6068,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>506</v>
       </c>
@@ -6094,7 +6094,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>507</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>508</v>
       </c>
@@ -6146,7 +6146,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>509</v>
       </c>
@@ -6172,7 +6172,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>510</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>511</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>494</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>496</v>
       </c>
@@ -6276,7 +6276,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>498</v>
       </c>
@@ -6302,7 +6302,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>500</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>501</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>502</v>
       </c>
@@ -6380,7 +6380,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>125</v>
       </c>
@@ -6412,7 +6412,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>154</v>
       </c>
@@ -6444,7 +6444,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -6514,7 +6514,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>122</v>
       </c>
@@ -6534,7 +6534,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>123</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>124</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>151</v>
       </c>
@@ -6594,7 +6594,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>152</v>
       </c>
@@ -6614,7 +6614,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>153</v>
       </c>
@@ -6634,7 +6634,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>126</v>
       </c>
@@ -6657,7 +6657,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>127</v>
       </c>
@@ -6680,7 +6680,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>128</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>155</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>156</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>157</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>555</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>557</v>
       </c>
@@ -6842,7 +6842,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>558</v>
       </c>
@@ -6865,7 +6865,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>561</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>562</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>563</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>129</v>
       </c>
@@ -6957,7 +6957,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>158</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>53</v>
       </c>
@@ -7003,7 +7003,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>313</v>
       </c>
@@ -7020,7 +7020,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>569</v>
       </c>
@@ -7043,7 +7043,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>572</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>576</v>
       </c>
@@ -7089,7 +7089,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>578</v>
       </c>
@@ -7112,7 +7112,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>584</v>
       </c>
@@ -7135,7 +7135,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>586</v>
       </c>
@@ -7158,7 +7158,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>588</v>
       </c>
@@ -7181,7 +7181,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>570</v>
       </c>
@@ -7204,7 +7204,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>574</v>
       </c>
@@ -7227,7 +7227,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>577</v>
       </c>
@@ -7250,7 +7250,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>579</v>
       </c>
@@ -7273,7 +7273,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>585</v>
       </c>
@@ -7296,7 +7296,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>587</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>589</v>
       </c>
@@ -7344,11 +7344,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -7356,11 +7351,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
@@ -7375,7 +7370,7 @@
     <col min="15" max="15" width="75.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -7407,7 +7402,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -7430,7 +7425,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16" customHeight="1">
+    <row r="3" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>632</v>
       </c>
@@ -7451,7 +7446,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>272</v>
       </c>
@@ -7472,7 +7467,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="16" customHeight="1">
+    <row r="5" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>284</v>
       </c>
@@ -7493,7 +7488,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="16" customHeight="1">
+    <row r="6" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>285</v>
       </c>
@@ -7514,7 +7509,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>199</v>
       </c>
@@ -7537,7 +7532,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>209</v>
       </c>
@@ -7557,7 +7552,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>210</v>
       </c>
@@ -7577,7 +7572,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>211</v>
       </c>
@@ -7597,7 +7592,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>202</v>
       </c>
@@ -7617,7 +7612,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>212</v>
       </c>
@@ -7637,7 +7632,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>213</v>
       </c>
@@ -7657,7 +7652,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>214</v>
       </c>
@@ -7677,11 +7672,11 @@
         <v>285</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="J15" s="40"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>280</v>
       </c>
@@ -7702,7 +7697,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>267</v>
       </c>
@@ -7723,7 +7718,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="16" customHeight="1">
+    <row r="18" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>268</v>
       </c>
@@ -7744,7 +7739,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>222</v>
       </c>
@@ -7765,7 +7760,7 @@
       </c>
       <c r="I19" s="23"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>223</v>
       </c>
@@ -7785,7 +7780,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>198</v>
       </c>
@@ -7805,7 +7800,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>200</v>
       </c>
@@ -7825,7 +7820,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>201</v>
       </c>
@@ -7845,7 +7840,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>203</v>
       </c>
@@ -7865,10 +7860,10 @@
         <v>267</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>264</v>
       </c>
@@ -7892,7 +7887,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>265</v>
       </c>
@@ -7916,7 +7911,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>266</v>
       </c>
@@ -7940,7 +7935,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>130</v>
       </c>
@@ -7961,7 +7956,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="28">
+    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>258</v>
       </c>
@@ -7985,7 +7980,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="42">
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="43" t="s">
         <v>292</v>
       </c>
@@ -8009,7 +8004,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="43" t="s">
         <v>293</v>
       </c>
@@ -8033,7 +8028,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -8054,7 +8049,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -8075,7 +8070,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>159</v>
       </c>
@@ -8096,7 +8091,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>160</v>
       </c>
@@ -8117,7 +8112,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>161</v>
       </c>
@@ -8138,7 +8133,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>259</v>
       </c>
@@ -8156,7 +8151,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -8177,7 +8172,7 @@
       </c>
       <c r="I39" s="23"/>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -8197,7 +8192,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>66</v>
       </c>
@@ -8217,7 +8212,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>67</v>
       </c>
@@ -8237,11 +8232,11 @@
         <v>286</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B43" s="2"/>
       <c r="H43"/>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>251</v>
       </c>
@@ -8264,7 +8259,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -8288,10 +8283,10 @@
       </c>
       <c r="J45" s="23"/>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:15" ht="28">
+    <row r="47" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>596</v>
       </c>
@@ -8313,7 +8308,7 @@
       </c>
       <c r="O47" s="2"/>
     </row>
-    <row r="48" spans="1:15" ht="28">
+    <row r="48" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>597</v>
       </c>
@@ -8335,7 +8330,7 @@
       </c>
       <c r="O48" s="2"/>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>598</v>
       </c>
@@ -8357,7 +8352,7 @@
       </c>
       <c r="O49" s="2"/>
     </row>
-    <row r="50" spans="1:15" ht="28">
+    <row r="50" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>599</v>
       </c>
@@ -8379,7 +8374,7 @@
       </c>
       <c r="O50" s="2"/>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>600</v>
       </c>
@@ -8401,7 +8396,7 @@
       </c>
       <c r="O51" s="2"/>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>601</v>
       </c>
@@ -8423,7 +8418,7 @@
       </c>
       <c r="O52" s="2"/>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>602</v>
       </c>
@@ -8440,7 +8435,7 @@
       </c>
       <c r="O53" s="2"/>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>603</v>
       </c>
@@ -8457,7 +8452,7 @@
       </c>
       <c r="O54" s="2"/>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>133</v>
       </c>
@@ -8474,7 +8469,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>162</v>
       </c>
@@ -8491,7 +8486,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>134</v>
       </c>
@@ -8508,7 +8503,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>135</v>
       </c>
@@ -8525,7 +8520,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>136</v>
       </c>
@@ -8542,7 +8537,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>163</v>
       </c>
@@ -8560,7 +8555,7 @@
       </c>
       <c r="J60" s="23"/>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>164</v>
       </c>
@@ -8578,7 +8573,7 @@
       </c>
       <c r="J61" s="23"/>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>165</v>
       </c>
@@ -8596,12 +8591,12 @@
       </c>
       <c r="J62" s="23"/>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B63" s="2"/>
       <c r="C63" s="43"/>
       <c r="J63" s="23"/>
     </row>
-    <row r="64" spans="1:15" ht="28">
+    <row r="64" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>137</v>
       </c>
@@ -8627,7 +8622,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>138</v>
       </c>
@@ -8656,7 +8651,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>139</v>
       </c>
@@ -8685,7 +8680,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>140</v>
       </c>
@@ -8714,7 +8709,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="28">
+    <row r="68" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>142</v>
       </c>
@@ -8740,7 +8735,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>143</v>
       </c>
@@ -8769,7 +8764,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>144</v>
       </c>
@@ -8798,7 +8793,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>145</v>
       </c>
@@ -8827,7 +8822,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="28">
+    <row r="72" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>147</v>
       </c>
@@ -8853,7 +8848,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>148</v>
       </c>
@@ -8879,7 +8874,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>149</v>
       </c>
@@ -8905,7 +8900,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>150</v>
       </c>
@@ -8931,7 +8926,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="28">
+    <row r="76" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>166</v>
       </c>
@@ -8957,7 +8952,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>167</v>
       </c>
@@ -8986,7 +8981,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>168</v>
       </c>
@@ -9015,7 +9010,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>169</v>
       </c>
@@ -9044,7 +9039,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="28">
+    <row r="80" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>171</v>
       </c>
@@ -9070,7 +9065,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>172</v>
       </c>
@@ -9099,7 +9094,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>173</v>
       </c>
@@ -9128,7 +9123,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>174</v>
       </c>
@@ -9157,7 +9152,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="28">
+    <row r="84" spans="1:15" ht="30" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>176</v>
       </c>
@@ -9183,7 +9178,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>177</v>
       </c>
@@ -9209,7 +9204,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>178</v>
       </c>
@@ -9235,7 +9230,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>179</v>
       </c>
@@ -9261,11 +9256,11 @@
         <v>622</v>
       </c>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B88" s="2"/>
       <c r="J88" s="2"/>
     </row>
-    <row r="89" spans="1:15" ht="56">
+    <row r="89" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>300</v>
       </c>
@@ -9291,7 +9286,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="42">
+    <row r="90" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>297</v>
       </c>
@@ -9320,7 +9315,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>298</v>
       </c>
@@ -9346,7 +9341,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="92" spans="1:15">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>299</v>
       </c>
@@ -9372,7 +9367,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="93" spans="1:15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>302</v>
       </c>
@@ -9398,7 +9393,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="94" spans="1:15">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>301</v>
       </c>
@@ -9424,7 +9419,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="95" spans="1:15">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>170</v>
       </c>
@@ -9445,7 +9440,7 @@
       </c>
       <c r="J95" s="23"/>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>175</v>
       </c>
@@ -9466,7 +9461,7 @@
       </c>
       <c r="J96" s="23"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>141</v>
       </c>
@@ -9487,7 +9482,7 @@
       </c>
       <c r="J97" s="23"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>146</v>
       </c>
@@ -9508,11 +9503,11 @@
       </c>
       <c r="J98" s="23"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B99" s="2"/>
       <c r="J99" s="23"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>413</v>
       </c>
@@ -9535,7 +9530,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>414</v>
       </c>
@@ -9558,7 +9553,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>415</v>
       </c>
@@ -9581,7 +9576,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>410</v>
       </c>
@@ -9610,7 +9605,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>411</v>
       </c>
@@ -9639,7 +9634,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>412</v>
       </c>
@@ -9665,7 +9660,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>416</v>
       </c>
@@ -9688,7 +9683,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>417</v>
       </c>
@@ -9711,7 +9706,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>418</v>
       </c>
@@ -9734,7 +9729,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>419</v>
       </c>
@@ -9763,7 +9758,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>420</v>
       </c>
@@ -9792,7 +9787,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>421</v>
       </c>
@@ -9818,27 +9813,22 @@
         <v>618</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B112" s="2"/>
       <c r="J112" s="2"/>
     </row>
-    <row r="113" spans="10:10">
+    <row r="113" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J113" s="49"/>
     </row>
-    <row r="114" spans="10:10">
+    <row r="114" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J114" s="49"/>
     </row>
-    <row r="115" spans="10:10">
+    <row r="115" spans="10:10" x14ac:dyDescent="0.2">
       <c r="J115" s="50"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -9850,22 +9840,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="77" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>246</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Attempts for Demographic Fit
Calculations mentioned in the e-mail are in the databook-belarus sheet,
with the perfect scenario of 0 difference left to see and compare
against the original values below.

Updated the SP Untreated Death rates in the cascade sheet according to
Lara’s e-mail.

Line added to project/run_belarus.py by David to change time-step to 1
temporarily for these test runs, and 1995 start date changed to 2000.

Hoping this is clear!
</commit_message>
<xml_diff>
--- a/project/cascade-belarus.xlsx
+++ b/project/cascade-belarus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25040" windowHeight="14960" tabRatio="647" activeTab="4"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25040" windowHeight="14960" tabRatio="647" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Sheet Names" sheetId="5" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Parameters" sheetId="3" r:id="rId5"/>
     <sheet name="Notes" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" calcMode="autoNoTable" iterate="1" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="635">
   <si>
     <t>Code Label</t>
   </si>
@@ -5647,8 +5647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="C30" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5730,6 +5730,9 @@
       <c r="I2" t="s">
         <v>3</v>
       </c>
+      <c r="O2" s="2" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
@@ -6535,6 +6538,9 @@
       <c r="K36" t="s">
         <v>153</v>
       </c>
+      <c r="O36" s="2" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" t="s">
@@ -6572,9 +6578,6 @@
       </c>
       <c r="N38" t="s">
         <v>50</v>
-      </c>
-      <c r="O38" s="2" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -7419,7 +7422,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -9902,7 +9905,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Previous cascade had not saved
This is the most current cascade, please ignore previous version which
had not saved with Lara’s change.
</commit_message>
<xml_diff>
--- a/project/cascade-belarus.xlsx
+++ b/project/cascade-belarus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="25040" windowHeight="14960" tabRatio="647" activeTab="3"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="25040" windowHeight="14960" tabRatio="647" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Databook Sheet Names" sheetId="5" r:id="rId1"/>
@@ -5647,7 +5647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C30" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="O39" sqref="O39"/>
     </sheetView>
   </sheetViews>
@@ -7422,8 +7422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106:D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -9595,7 +9595,7 @@
         <v>436</v>
       </c>
       <c r="D100" s="2">
-        <v>0.7</v>
+        <v>0.12</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>448</v>
@@ -9618,7 +9618,7 @@
         <v>437</v>
       </c>
       <c r="D101" s="2">
-        <v>0.7</v>
+        <v>0.12</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>448</v>
@@ -9641,7 +9641,7 @@
         <v>438</v>
       </c>
       <c r="D102" s="2">
-        <v>0.7</v>
+        <v>0.12</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>448</v>
@@ -9747,7 +9747,7 @@
       <c r="C106" s="43" t="s">
         <v>445</v>
       </c>
-      <c r="D106" s="2">
+      <c r="D106" s="54">
         <v>0.2</v>
       </c>
       <c r="E106" s="2" t="s">
@@ -9770,7 +9770,7 @@
       <c r="C107" s="43" t="s">
         <v>446</v>
       </c>
-      <c r="D107" s="2">
+      <c r="D107" s="54">
         <v>0.2</v>
       </c>
       <c r="E107" s="2" t="s">
@@ -9793,7 +9793,7 @@
       <c r="C108" s="43" t="s">
         <v>447</v>
       </c>
-      <c r="D108" s="2">
+      <c r="D108" s="54">
         <v>0.2</v>
       </c>
       <c r="E108" s="2" t="s">

</xml_diff>